<commit_message>
Updated FA1 BOM - Added receptacle and pins for board connectors
</commit_message>
<xml_diff>
--- a/sch/FA1/FA1_BOM.xlsx
+++ b/sch/FA1/FA1_BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -164,6 +164,42 @@
   </si>
   <si>
     <t xml:space="preserve">Jaycar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HOUSING VH 2POS 3.96MM WHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455-1183-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VHR-2N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN HOUSING VH 3POS 3.96MM WHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455-1184-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VHR-3N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN TERM CRIMP VH/NV 18-22AWG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455-1133-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVH-21T-P1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used for LEDs, IEC, SMA and DMX</t>
   </si>
   <si>
     <t xml:space="preserve">ANT LTE BLADE SWIVEL DIPOLE SMA</t>
@@ -521,10 +557,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -536,7 +572,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -828,14 +864,14 @@
         <v>15</v>
       </c>
       <c r="G10" s="16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" s="17" t="n">
-        <v>13.62</v>
+        <v>0.17</v>
       </c>
       <c r="I10" s="17" t="n">
         <f aca="false">H10*G10</f>
-        <v>13.62</v>
+        <v>0.51</v>
       </c>
       <c r="J10" s="15"/>
     </row>
@@ -844,81 +880,108 @@
       <c r="B11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
+      <c r="C11" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="G11" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="H11" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="17" t="n">
+        <v>0.2</v>
+      </c>
       <c r="I11" s="17" t="n">
         <f aca="false">H11*G11</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="G12" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="H12" s="17"/>
+        <v>9</v>
+      </c>
+      <c r="H12" s="17" t="n">
+        <v>0.16</v>
+      </c>
       <c r="I12" s="17" t="n">
         <f aca="false">H12*G12</f>
-        <v>0</v>
+        <v>1.44</v>
       </c>
       <c r="J12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="16" t="n">
-        <v>4</v>
-      </c>
+      <c r="G13" s="16"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="17" t="n">
-        <f aca="false">H13*G13</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="15"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="G14" s="16" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" s="17"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="17" t="n">
+        <v>13.62</v>
+      </c>
       <c r="I14" s="17" t="n">
         <f aca="false">H14*G14</f>
-        <v>0</v>
+        <v>13.62</v>
       </c>
       <c r="J14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -937,74 +1000,138 @@
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="16" t="n">
-        <v>1780002</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>15</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="17" t="n">
-        <v>8.88</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H16" s="17"/>
       <c r="I16" s="17" t="n">
         <f aca="false">H16*G16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17" t="n">
+        <f aca="false">H17*G17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17" t="n">
+        <f aca="false">H18*G18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16" t="n">
+        <v>4</v>
+      </c>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17" t="n">
+        <f aca="false">H19*G19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="16" t="n">
+        <v>1780002</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="17" t="n">
         <v>8.88</v>
       </c>
-      <c r="J16" s="15"/>
-    </row>
-    <row r="17" s="23" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="20" t="s">
+      <c r="I20" s="17" t="n">
+        <f aca="false">H20*G20</f>
+        <v>8.88</v>
+      </c>
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" s="23" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18"/>
+      <c r="B21" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="21" t="n">
+      <c r="G21" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="21" t="n">
         <v>8.02</v>
       </c>
-      <c r="I17" s="21" t="n">
-        <f aca="false">H17*G17</f>
+      <c r="I21" s="21" t="n">
+        <f aca="false">H21*G21</f>
         <v>8.02</v>
       </c>
-      <c r="J17" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G21" s="1"/>
+      <c r="J21" s="22" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G22" s="1"/>
@@ -1015,13 +1142,25 @@
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="I31" s="25" t="n">
-        <f aca="false">SUM(I4:I17)</f>
-        <v>84.73</v>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H35" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I35" s="25" t="n">
+        <f aca="false">SUM(I4:I21)</f>
+        <v>86.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>